<commit_message>
resultados y no tan resultados
</commit_message>
<xml_diff>
--- a/results/resumenResultados.xlsx
+++ b/results/resumenResultados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="orinaFlav" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>sexoF</t>
   </si>
@@ -74,6 +74,69 @@
   </si>
   <si>
     <t>anova 2/3 vias</t>
+  </si>
+  <si>
+    <t>Distribución muy dispersa</t>
+  </si>
+  <si>
+    <t>Distribución concentrada</t>
+  </si>
+  <si>
+    <t>Distribución menos concentrada</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Muy disperso</t>
+  </si>
+  <si>
+    <t>Disperso</t>
+  </si>
+  <si>
+    <t>Muy disperso, alta variabilidad y alta media ES y NS, Sexo/end equilibrado</t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>ES, NG</t>
+  </si>
+  <si>
+    <t>Delta.Frec, Delta.Grasa</t>
+  </si>
+  <si>
+    <t>Concentrado, poca variabilidad, equilibrado en factores</t>
+  </si>
+  <si>
+    <t>Concentrado, valor medio bajo de ES, de HE.G, de NG y NS, antro normal, Casi todo hombres</t>
+  </si>
+  <si>
+    <t>Sexo H, ES, HE.G, NG, NS</t>
+  </si>
+  <si>
+    <t>Disperso, valor muy alto y distinto de HE.G, parecido NG,  + Sa, casi todo mujeres</t>
+  </si>
+  <si>
+    <t>Sexo M, HE.G, NG, SA</t>
+  </si>
+  <si>
+    <t>Muy disperso niveles bajos de EG, HE.G, NG, baja media de peso, baja media de grasa, baja medai delta.IRCV, baja media Bpmx, casi todo hombre, + ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sexo H, EG, HE.G, NG, peso, grasa IRCV, BPMAX, ST, </t>
+  </si>
+  <si>
+    <t>Concentrado y definido</t>
+  </si>
+  <si>
+    <t>Definido algo disperso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentrado y definido, poca variabilidad, mayoría ST/SU, </t>
   </si>
 </sst>
 </file>
@@ -109,11 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,16 +458,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
   </cols>
@@ -455,46 +519,119 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>3</v>
       </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -504,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,28 +697,64 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -590,9 +763,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>